<commit_message>
finished count vs time plots for 3 scenarios
</commit_message>
<xml_diff>
--- a/3scenarios/error/ErrorVsTime_S1.xlsx
+++ b/3scenarios/error/ErrorVsTime_S1.xlsx
@@ -18,13 +18,14 @@
     <sheet name="T9" sheetId="9" r:id="rId9"/>
     <sheet name="T10" sheetId="10" r:id="rId10"/>
     <sheet name="Average" sheetId="11" r:id="rId11"/>
+    <sheet name="CountVsTime" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>PI(t)D(t) Time</t>
   </si>
@@ -36,6 +37,36 @@
   </si>
   <si>
     <t>PI(t)D(t) Avg Error</t>
+  </si>
+  <si>
+    <t>PI(t)D(t) Time Interval</t>
+  </si>
+  <si>
+    <t>PI(t)D(t) Count</t>
+  </si>
+  <si>
+    <t>2781-2854</t>
+  </si>
+  <si>
+    <t>2855-2929</t>
+  </si>
+  <si>
+    <t>2930-3004</t>
+  </si>
+  <si>
+    <t>3005-3079</t>
+  </si>
+  <si>
+    <t>3080-3154</t>
+  </si>
+  <si>
+    <t>3155-3229</t>
+  </si>
+  <si>
+    <t>3230-3304</t>
+  </si>
+  <si>
+    <t>3305-3379</t>
   </si>
 </sst>
 </file>
@@ -21765,6 +21796,350 @@
         <c:crossAx val="50110001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Count vs Time
+Scenario 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14000000000000001"/>
+          <c:y val="0.20000000000000001"/>
+          <c:w val="0.81999999999999995"/>
+          <c:h val="0.5"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="BF0000"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountVsTime!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2781-2854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2855-2929</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2930-3004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3005-3079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3080-3154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3155-3229</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3230-3304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3305-3379</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountVsTime!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50120001"/>
+        <c:axId val="50120002"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="700000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="700000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="700000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountVsTime!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2781-2854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2855-2929</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2930-3004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3005-3079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3080-3154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3155-3229</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3230-3304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3305-3379</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountVsTime!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50120001"/>
+        <c:axId val="50120002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50120001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time To Reach Target (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50120002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50120002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50120001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -30728,6 +31103,41 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -70022,6 +70432,116 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C142"/>

</xml_diff>